<commit_message>
Sequential execution of test case with threadsafety
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/UpdateEmployeeData.xlsx
+++ b/src/test/resources/Data/UpdateEmployeeData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarit\eclipse-workspace\employee-api-tests\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarit\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED15D187-22E8-4F46-8060-A18117C529A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EC1D151-5223-46BD-B2A0-3D7CA216CB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0B7B5AE-6266-4CA6-9D41-6C5D1CADB66D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74EFBB53-BC22-4E4D-B788-5C4414BDF000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdateEmployee" sheetId="1" r:id="rId1"/>
@@ -35,42 +35,11 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Saritha m</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0F2DABB8-57D9-4B7D-94E1-46C527D592A0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Saritha m:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Method name</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>validateValidEmployeeUpdate</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -78,80 +47,35 @@
     <t>job</t>
   </si>
   <si>
-    <t>jjk</t>
-  </si>
-  <si>
-    <t>testGetUserDataSuccess</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>avatar</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>janet.weaver@reqres.in</t>
-  </si>
-  <si>
-    <t>Janet</t>
-  </si>
-  <si>
-    <t>Weaver</t>
-  </si>
-  <si>
-    <t>https://reqres.in/img/faces/2-image.jpg</t>
-  </si>
-  <si>
-    <t>https://reqres.in/#support-heading</t>
-  </si>
-  <si>
-    <t>To keep ReqRes free, contributions towards server costs are appreciated!</t>
-  </si>
-  <si>
-    <t>validateValidEmployeeUpdate</t>
-  </si>
-  <si>
     <t>morpheus</t>
   </si>
   <si>
-    <t>leader</t>
+    <t>zion resident</t>
   </si>
   <si>
     <t>validateInvalidEmployeeIdUpdate</t>
   </si>
   <si>
-    <t>"$%%%</t>
+    <t>$%^</t>
+  </si>
+  <si>
+    <t>*&amp;^</t>
   </si>
   <si>
     <t>validateInvalidEmployeeDataUpdate</t>
   </si>
   <si>
-    <t>^&amp;**</t>
-  </si>
-  <si>
-    <t>#$$%%</t>
+    <t>Manju</t>
+  </si>
+  <si>
+    <t>Dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,55 +86,26 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF312540"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF445797"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,35 +131,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,146 +475,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A45579F-8418-422F-8A3E-20D8E5EF5099}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E1C71-885E-49EC-A656-02DE68FFAD47}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.109375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" location="support-heading" display="https://reqres.in/ - support-heading" xr:uid="{8362B298-2848-42B2-A886-1953EE2D9DF7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>